<commit_message>
4.4 and 7.1 notes finished
</commit_message>
<xml_diff>
--- a/Stat5100/course/S20 Schedule (Stat 5100) - adjusted.xlsx
+++ b/Stat5100/course/S20 Schedule (Stat 5100) - adjusted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E80E314-B24D-4CF7-BAE8-25394F497E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7126C1EC-03C7-4FD7-9A6D-D93C2BEB788B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,14 +411,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +702,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -714,11 +714,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -1027,7 +1027,7 @@
       <c r="A33" s="4">
         <v>43906</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="24" t="s">
         <v>51</v>
       </c>
       <c r="C33" s="5"/>
@@ -1055,7 +1055,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="26">
+      <c r="A36" s="25">
         <v>43913</v>
       </c>
       <c r="B36" s="14" t="s">
@@ -1066,19 +1066,19 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="26">
+      <c r="A37" s="25">
         <v>43915</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="28"/>
+      <c r="C37" s="27"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="26">
+      <c r="A38" s="25">
         <v>43917</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="28" t="s">
         <v>51</v>
       </c>
       <c r="C38" s="12" t="s">
@@ -1117,28 +1117,28 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="26">
+      <c r="A42" s="25">
         <v>43927</v>
       </c>
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="28" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="12"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="26">
+      <c r="A43" s="25">
         <v>43929</v>
       </c>
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="28" t="s">
         <v>51</v>
       </c>
       <c r="C43" s="14"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="26">
+      <c r="A44" s="25">
         <v>43931</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="26" t="s">
         <v>50</v>
       </c>
       <c r="C44" s="16" t="s">
@@ -1187,7 +1187,7 @@
       <c r="A49" s="2">
         <v>43943</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="12" t="s">

</xml_diff>

<commit_message>
notes through module 5
</commit_message>
<xml_diff>
--- a/Stat5100/course/S20 Schedule (Stat 5100) - adjusted.xlsx
+++ b/Stat5100/course/S20 Schedule (Stat 5100) - adjusted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7126C1EC-03C7-4FD7-9A6D-D93C2BEB788B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4784DE2-E15A-4104-8B74-EABFE92C2A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -181,12 +181,6 @@
     <t>6.2: Time Series Case Study</t>
   </si>
   <si>
-    <t xml:space="preserve">HW 6/Final Project Papers - First Draft </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HW 7/Review Response/Final Project Papers - Final Draft </t>
-  </si>
-  <si>
     <t>4.3: Model Validation</t>
   </si>
   <si>
@@ -211,18 +205,12 @@
     <t xml:space="preserve">Quiz 4 </t>
   </si>
   <si>
-    <t>Quiz 5</t>
-  </si>
-  <si>
     <t>D.2 Group Work Primer (make up)</t>
   </si>
   <si>
     <t>HW 4/Project 2 Papers - First Draft</t>
   </si>
   <si>
-    <t>HW 5/Project 2 Papers - Final Draft</t>
-  </si>
-  <si>
     <t>Final Project Proposals</t>
   </si>
   <si>
@@ -269,13 +257,37 @@
   </si>
   <si>
     <t>Final Project Paper Update</t>
+  </si>
+  <si>
+    <t>HW 5</t>
+  </si>
+  <si>
+    <t>Project 2 Papers - Final Draft</t>
+  </si>
+  <si>
+    <t>HW 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 5  </t>
+  </si>
+  <si>
+    <t>Final Project Papers - First Draft</t>
+  </si>
+  <si>
+    <t>HW 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review Response/Final Project Papers - Final Draft </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monday of Finals Week </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +342,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -378,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -416,9 +436,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +727,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -714,11 +739,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -862,7 +887,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -922,7 +947,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -933,7 +958,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -964,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -999,7 +1024,7 @@
         <v>43899</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C30" s="6"/>
     </row>
@@ -1008,7 +1033,7 @@
         <v>43901</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C31" s="11"/>
     </row>
@@ -1017,10 +1042,10 @@
         <v>43903</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1028,7 +1053,7 @@
         <v>43906</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C33" s="5"/>
     </row>
@@ -1037,10 +1062,10 @@
         <v>43908</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1048,10 +1073,10 @@
         <v>43910</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1059,10 +1084,10 @@
         <v>43913</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1070,7 +1095,7 @@
         <v>43915</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C37" s="27"/>
     </row>
@@ -1079,10 +1104,10 @@
         <v>43917</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1090,19 +1115,21 @@
         <v>43920</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>43922</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1112,25 +1139,25 @@
       <c r="B41" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="C41" s="10"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="25">
         <v>43927</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="25">
         <v>43929</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C43" s="14"/>
     </row>
@@ -1139,10 +1166,10 @@
         <v>43931</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1150,7 +1177,7 @@
         <v>43934</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C45" s="10"/>
     </row>
@@ -1161,8 +1188,8 @@
       <c r="B46" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="10" t="s">
-        <v>44</v>
+      <c r="C46" s="32" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1170,16 +1197,18 @@
         <v>43938</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>43941</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C48" s="12"/>
     </row>
@@ -1191,7 +1220,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1199,10 +1228,21 @@
         <v>43945</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>35</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="34">
+        <v>43948</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1215,7 +1255,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all the teaching notes
</commit_message>
<xml_diff>
--- a/Stat5100/course/S20 Schedule (Stat 5100) - adjusted.xlsx
+++ b/Stat5100/course/S20 Schedule (Stat 5100) - adjusted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4784DE2-E15A-4104-8B74-EABFE92C2A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79194799-8BAD-4E8B-B175-F139634F0406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38770" yWindow="1130" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,9 +175,6 @@
     <t>3.3: Model Influence</t>
   </si>
   <si>
-    <t>5.2: Extensions of Logistic Regression</t>
-  </si>
-  <si>
     <t>6.2: Time Series Case Study</t>
   </si>
   <si>
@@ -281,6 +278,10 @@
   </si>
   <si>
     <t xml:space="preserve">Monday of Finals Week </t>
+  </si>
+  <si>
+    <t>5.2 Multi-Class Logisitic Regression
+5.3: Logistic Regression Case Study</t>
   </si>
 </sst>
 </file>
@@ -398,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -438,12 +439,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -739,11 +743,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
@@ -887,7 +891,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -947,7 +951,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -958,7 +962,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -989,7 +993,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1024,7 +1028,7 @@
         <v>43899</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="6"/>
     </row>
@@ -1033,7 +1037,7 @@
         <v>43901</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="11"/>
     </row>
@@ -1042,10 +1046,10 @@
         <v>43903</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1053,7 +1057,7 @@
         <v>43906</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="5"/>
     </row>
@@ -1062,10 +1066,10 @@
         <v>43908</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1073,10 +1077,10 @@
         <v>43910</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1084,10 +1088,10 @@
         <v>43913</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1095,7 +1099,7 @@
         <v>43915</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="27"/>
     </row>
@@ -1104,10 +1108,10 @@
         <v>43917</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1115,10 +1119,10 @@
         <v>43920</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1126,18 +1130,18 @@
         <v>43922</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>43924</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>32</v>
+      <c r="B41" s="35" t="s">
+        <v>67</v>
       </c>
       <c r="C41" s="10"/>
     </row>
@@ -1146,10 +1150,10 @@
         <v>43927</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1157,7 +1161,7 @@
         <v>43929</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" s="14"/>
     </row>
@@ -1166,10 +1170,10 @@
         <v>43931</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1177,7 +1181,7 @@
         <v>43934</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" s="10"/>
     </row>
@@ -1186,10 +1190,10 @@
         <v>43936</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" s="32" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1197,10 +1201,10 @@
         <v>43938</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1208,7 +1212,7 @@
         <v>43941</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="12"/>
     </row>
@@ -1220,7 +1224,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1228,21 +1232,21 @@
         <v>43945</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="33">
+        <v>43948</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="32" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="34">
-        <v>43948</v>
-      </c>
-      <c r="B51" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="33" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1255,7 +1259,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>